<commit_message>
all training texts cleaned
</commit_message>
<xml_diff>
--- a/Project_python/out/results4.xlsx
+++ b/Project_python/out/results4.xlsx
@@ -486,7 +486,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[0.014840159163238213]</t>
+          <t>[0.017432467615872395]</t>
         </is>
       </c>
       <c r="F2" t="b">
@@ -517,7 +517,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[0.050499359328172184]</t>
+          <t>[0.044403652986481974]</t>
         </is>
       </c>
       <c r="F3" t="b">
@@ -548,7 +548,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[0.024337665768051034, 0.01714352098382592]</t>
+          <t>[0.024536868481554435, 0.015611969252747153]</t>
         </is>
       </c>
       <c r="F4" t="b">
@@ -579,7 +579,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[0.05241817128926408]</t>
+          <t>[0.04833103438705824]</t>
         </is>
       </c>
       <c r="F5" t="b">
@@ -610,7 +610,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[0.053077686025112016]</t>
+          <t>[0.04932457982596433]</t>
         </is>
       </c>
       <c r="F6" t="b">
@@ -641,7 +641,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[0.029409252575383866]</t>
+          <t>[0.025772738900568224]</t>
         </is>
       </c>
       <c r="F7" t="b">
@@ -672,7 +672,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[0.06537741687979529]</t>
+          <t>[0.05917762990122566]</t>
         </is>
       </c>
       <c r="F8" t="b">
@@ -703,7 +703,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[0.07584364532836234]</t>
+          <t>[0.07702890905447025]</t>
         </is>
       </c>
       <c r="F9" t="b">
@@ -734,7 +734,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[0.03779795845399963]</t>
+          <t>[0.037373281837366316]</t>
         </is>
       </c>
       <c r="F10" t="b">
@@ -765,7 +765,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[0.08848636224196181]</t>
+          <t>[0.08214139872170138]</t>
         </is>
       </c>
       <c r="F11" t="b">
@@ -781,29 +781,29 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>[15]</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>inadequacy spatial soil information limiting factor making evidence based decision improve food security land management developing country digital soil mapping dsm technique applied world improve availability usability soil africa particularly tanzania scale necessary farm management decision kilombero valley identified intensified rice production valley lack detailed todate soil information decision making overall objective study develop predictive soil map portion kilombero valley dsm technique widely decision tree algorithm source digital elevation model dems evaluated predictive ability firstly numerical classification performed collected soil profile arrive soil taxon secondly derived taxon spatially predicted mapped following scorpan framework random forest machine learning algorithm datasets train model derived legacy soil map rapideye satellite image dems arc srtm aster worlddem separate predictive model built dem source mapping showed sensitive training set sampling result showed prediction soil taxon arc srtm worddem identical suggest algorithm freely available srtm dem combination mapping soil kilombero valley combination tested applied area relatively flat terrain like kilombero valley</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>[2]</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>inadequacy spatial soil information limiting factor making evidence based decision improve food security land management developing country digital soil mapping dsm technique applied world improve availability usability soil africa particularly tanzania scale necessary farm management decision kilombero valley identified intensified rice production valley lack detailed todate soil information decision making overall objective study develop predictive soil map portion kilombero valley dsm technique widely decision tree algorithm source digital elevation model dems evaluated predictive ability firstly numerical classification performed collected soil profile arrive soil taxon secondly derived taxon spatially predicted mapped following scorpan framework random forest machine learning algorithm datasets train model derived legacy soil map rapideye satellite image dems arc srtm aster worlddem separate predictive model built dem source mapping showed sensitive training set sampling result showed prediction soil taxon arc srtm worddem identical suggest algorithm freely available srtm dem combination mapping soil kilombero valley combination tested applied area relatively flat terrain like kilombero valley</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>[2]</t>
-        </is>
-      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>[0.032652133822185035]</t>
+          <t>[0.040706005820995796]</t>
         </is>
       </c>
       <c r="F12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -827,7 +827,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[0.04848807105428687]</t>
+          <t>[0.045565301537595845]</t>
         </is>
       </c>
       <c r="F13" t="b">
@@ -858,7 +858,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[0.049266701759172915]</t>
+          <t>[0.048014534869808514]</t>
         </is>
       </c>
       <c r="F14" t="b">
@@ -889,7 +889,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>[0.014496618818782865, 0.006923125176686368]</t>
+          <t>[0.015323597332810666, 0.007830188437992823]</t>
         </is>
       </c>
       <c r="F15" t="b">
@@ -920,7 +920,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[0.06769635823523502]</t>
+          <t>[0.06992478266892325]</t>
         </is>
       </c>
       <c r="F16" t="b">
@@ -951,7 +951,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>[0.0490583243726606]</t>
+          <t>[0.04308191972103614]</t>
         </is>
       </c>
       <c r="F17" t="b">
@@ -982,7 +982,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>[0.028173568320166646]</t>
+          <t>[0.02962054972952076]</t>
         </is>
       </c>
       <c r="F18" t="b">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[0.027475159529002223]</t>
+          <t>[0.02371407618005735]</t>
         </is>
       </c>
       <c r="F19" t="b">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>[0.02831276014701735, 0.025679766174111395]</t>
+          <t>[0.03876793373657218, 0.031187898744569887]</t>
         </is>
       </c>
       <c r="F20" t="b">
@@ -1060,7 +1060,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[5]</t>
+          <t>[15]</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>[0.01148436637375802]</t>
+          <t>[0.012500736368207714]</t>
         </is>
       </c>
       <c r="F21" t="b">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[0.020826378310266253]</t>
+          <t>[0.017978130719107147]</t>
         </is>
       </c>
       <c r="F22" t="b">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>[0.0414264965591381]</t>
+          <t>[0.03632008938380074]</t>
         </is>
       </c>
       <c r="F23" t="b">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[15]</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>[0.02146579763991265]</t>
+          <t>[0.017584882717591416]</t>
         </is>
       </c>
       <c r="F24" t="b">
@@ -1199,7 +1199,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[0.018579064871444676]</t>
+          <t>[0.017051619815027445]</t>
         </is>
       </c>
       <c r="F25" t="b">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[0.035002088350965556, 0.015736387071165807]</t>
+          <t>[0.0309614566552367, 0.01932710463698573]</t>
         </is>
       </c>
       <c r="F26" t="b">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[0.03257398061732888, 0.013418841821290573]</t>
+          <t>[0.02894130451873084, 0.012583833086087228]</t>
         </is>
       </c>
       <c r="F27" t="b">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>[0.03604293018675868]</t>
+          <t>[0.03772188784325417]</t>
         </is>
       </c>
       <c r="F28" t="b">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>[0.12027698426761704]</t>
+          <t>[0.12383055781358127]</t>
         </is>
       </c>
       <c r="F29" t="b">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>[0.014685962824674914]</t>
+          <t>[0.012407766384202844]</t>
         </is>
       </c>
       <c r="F30" t="b">
@@ -1385,7 +1385,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[0.023205800844013375, 0.0223230103586995]</t>
+          <t>[0.023094785434276965, 0.021985413720138118]</t>
         </is>
       </c>
       <c r="F31" t="b">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>[0.043620359992709766]</t>
+          <t>[0.03799026245323546]</t>
         </is>
       </c>
       <c r="F32" t="b">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>[0.020942427129065508]</t>
+          <t>[0.019176909653237144]</t>
         </is>
       </c>
       <c r="F33" t="b">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[0.04299031318027899]</t>
+          <t>[0.044391988487854195]</t>
         </is>
       </c>
       <c r="F34" t="b">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>[0.0547480042546068]</t>
+          <t>[0.05735350575610435]</t>
         </is>
       </c>
       <c r="F35" t="b">
@@ -1525,7 +1525,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[1]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1540,14 +1540,14 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>[0.030914050355180342]</t>
+          <t>[0.02934662774507949]</t>
         </is>
       </c>
       <c r="F36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[0.023659679990707783]</t>
+          <t>[0.0276601655942839]</t>
         </is>
       </c>
       <c r="F37" t="b">
@@ -1602,7 +1602,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>[0.01709293740717098]</t>
+          <t>[0.016732464004754193]</t>
         </is>
       </c>
       <c r="F38" t="b">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[0.03159476424391857]</t>
+          <t>[0.030980020677132545]</t>
         </is>
       </c>
       <c r="F39" t="b">
@@ -1664,7 +1664,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[0.015911631359791234]</t>
+          <t>[0.017730827140666733]</t>
         </is>
       </c>
       <c r="F40" t="b">
@@ -1695,7 +1695,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>[0.029395893489859513]</t>
+          <t>[0.030878906810104405]</t>
         </is>
       </c>
       <c r="F41" t="b">
@@ -1726,7 +1726,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>[0.02966241513432021]</t>
+          <t>[0.029623437339116907]</t>
         </is>
       </c>
       <c r="F42" t="b">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[0.04371992474434013]</t>
+          <t>[0.04480220132324833]</t>
         </is>
       </c>
       <c r="F43" t="b">
@@ -1788,7 +1788,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>[0.02458927101816065]</t>
+          <t>[0.022385449036099375]</t>
         </is>
       </c>
       <c r="F44" t="b">
@@ -1819,7 +1819,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>[0.012725215796150447]</t>
+          <t>[0.012377803764226149]</t>
         </is>
       </c>
       <c r="F45" t="b">
@@ -1835,7 +1835,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[13, 15]</t>
+          <t>[15, 13]</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1850,7 +1850,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[0.020207766455099127, 0.016525771924433184]</t>
+          <t>[0.022243809897753278, 0.01964642686971334]</t>
         </is>
       </c>
       <c r="F46" t="b">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>[0.020084267013013014]</t>
+          <t>[0.019670953936590015]</t>
         </is>
       </c>
       <c r="F47" t="b">
@@ -1912,7 +1912,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>[0.01517421121342288, 0.00993757331054094]</t>
+          <t>[0.015117169348878419, 0.011763728177526725]</t>
         </is>
       </c>
       <c r="F48" t="b">
@@ -1943,7 +1943,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[0.02260173991616746]</t>
+          <t>[0.01952576587753562]</t>
         </is>
       </c>
       <c r="F49" t="b">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>[0.05915268074473552]</t>
+          <t>[0.05198212705917045]</t>
         </is>
       </c>
       <c r="F50" t="b">
@@ -2005,7 +2005,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>[0.03414808908590349]</t>
+          <t>[0.030628624227837287]</t>
         </is>
       </c>
       <c r="F51" t="b">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[0.1141502436478766]</t>
+          <t>[0.10949024046393108]</t>
         </is>
       </c>
       <c r="F52" t="b">
@@ -2067,7 +2067,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>[0.046121864717057835]</t>
+          <t>[0.04438651542455275]</t>
         </is>
       </c>
       <c r="F53" t="b">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>[0.04295698666284836]</t>
+          <t>[0.0370854256985697]</t>
         </is>
       </c>
       <c r="F54" t="b">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>[0.04063391895116209]</t>
+          <t>[0.037521272059902265]</t>
         </is>
       </c>
       <c r="F55" t="b">
@@ -2160,7 +2160,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>[0.023908267178314808]</t>
+          <t>[0.022554075624907053]</t>
         </is>
       </c>
       <c r="F56" t="b">
@@ -2176,7 +2176,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>[0.01821058879897786]</t>
+          <t>[0.017484006881696032]</t>
         </is>
       </c>
       <c r="F57" t="b">
@@ -2222,7 +2222,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>[0.03279859249823352]</t>
+          <t>[0.030185192025332507]</t>
         </is>
       </c>
       <c r="F58" t="b">
@@ -2253,7 +2253,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>[0.028641308673402612]</t>
+          <t>[0.02821476451125166]</t>
         </is>
       </c>
       <c r="F59" t="b">
@@ -2284,7 +2284,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>[0.016458858616695122]</t>
+          <t>[0.014702574420562648]</t>
         </is>
       </c>
       <c r="F60" t="b">
@@ -2315,7 +2315,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>[0.09655680807321065]</t>
+          <t>[0.09658286070384246]</t>
         </is>
       </c>
       <c r="F61" t="b">
@@ -2331,7 +2331,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>[16]</t>
+          <t>[5]</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2346,14 +2346,14 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>[0.0330533278357935]</t>
+          <t>[0.032961232665122256]</t>
         </is>
       </c>
       <c r="F62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>[0.027927403260642147]</t>
+          <t>[0.026332242043221852]</t>
         </is>
       </c>
       <c r="F63" t="b">
@@ -2408,7 +2408,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>[0.03298668014746741]</t>
+          <t>[0.03255597927562634]</t>
         </is>
       </c>
       <c r="F64" t="b">
@@ -2439,7 +2439,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>[0.05594175619879136]</t>
+          <t>[0.05764494502179925]</t>
         </is>
       </c>
       <c r="F65" t="b">
@@ -2470,7 +2470,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>[0.023130886066589737]</t>
+          <t>[0.017621119048147928]</t>
         </is>
       </c>
       <c r="F66" t="b">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>[0.03464811973839797]</t>
+          <t>[0.03659541327304097]</t>
         </is>
       </c>
       <c r="F67" t="b">
@@ -2532,7 +2532,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>[0.06671547923065352]</t>
+          <t>[0.09404905795654304]</t>
         </is>
       </c>
       <c r="F68" t="b">
@@ -2563,7 +2563,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>[0.040786811805082875]</t>
+          <t>[0.04058786196749706]</t>
         </is>
       </c>
       <c r="F69" t="b">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>[0.06158680748401092]</t>
+          <t>[0.08441489805392428]</t>
         </is>
       </c>
       <c r="F70" t="b">
@@ -2625,7 +2625,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>[0.03306372605632121, 0.019345528864378018]</t>
+          <t>[0.03880385956173158, 0.01986489083894662]</t>
         </is>
       </c>
       <c r="F71" t="b">
@@ -2656,7 +2656,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>[0.16486011172498352]</t>
+          <t>[0.16510579343980775]</t>
         </is>
       </c>
       <c r="F72" t="b">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>[0.020182319522830502]</t>
+          <t>[0.01881610073201019]</t>
         </is>
       </c>
       <c r="F73" t="b">
@@ -2718,7 +2718,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>[0.024376913480900396]</t>
+          <t>[0.021146521631351004]</t>
         </is>
       </c>
       <c r="F74" t="b">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>[0.05397132134629108, 0.01883889680933482]</t>
+          <t>[0.04635685053197555, 0.0181426351237796]</t>
         </is>
       </c>
       <c r="F75" t="b">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[5]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2780,7 +2780,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>[0.020310597982571905]</t>
+          <t>[0.020854138931078008]</t>
         </is>
       </c>
       <c r="F76" t="b">
@@ -2811,7 +2811,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>[0.056544135834655625, 0.02220122392366542]</t>
+          <t>[0.048612828020562424, 0.022321241697399595]</t>
         </is>
       </c>
       <c r="F77" t="b">
@@ -2827,7 +2827,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[2]</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2842,7 +2842,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>[0.018049169195088463]</t>
+          <t>[0.012797368958357487]</t>
         </is>
       </c>
       <c r="F78" t="b">
@@ -2873,7 +2873,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>[0.04625217022460014]</t>
+          <t>[0.04686424172515893]</t>
         </is>
       </c>
       <c r="F79" t="b">
@@ -2904,7 +2904,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>[0.04388113665958206]</t>
+          <t>[0.04339757490094997]</t>
         </is>
       </c>
       <c r="F80" t="b">
@@ -2935,7 +2935,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>[0.11498477401738215, 0.021921868524742323]</t>
+          <t>[0.10706345118749275, 0.01769401646453737]</t>
         </is>
       </c>
       <c r="F81" t="b">
@@ -2966,7 +2966,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>[0.13843401547484194, 0.03355810747465617]</t>
+          <t>[0.14030418908329478, 0.03215802437884054]</t>
         </is>
       </c>
       <c r="F82" t="b">
@@ -2997,7 +2997,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>[0.027459173808269375, 0.018031417929509835]</t>
+          <t>[0.03208145317034763, 0.017905031648795755]</t>
         </is>
       </c>
       <c r="F83" t="b">
@@ -3013,7 +3013,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[8, 9]</t>
+          <t>[8, 14]</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3028,7 +3028,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>[0.039242434725776855, 0.02154368926575802]</t>
+          <t>[0.032694261021337434, 0.018308401127786204]</t>
         </is>
       </c>
       <c r="F84" t="b">
@@ -3059,7 +3059,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>[0.031488134036661244]</t>
+          <t>[0.028895844084202597]</t>
         </is>
       </c>
       <c r="F85" t="b">
@@ -3090,7 +3090,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>[0.019010520408641637]</t>
+          <t>[0.0188709140657014]</t>
         </is>
       </c>
       <c r="F86" t="b">
@@ -3106,7 +3106,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[5]</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>[0.02736101425502329]</t>
+          <t>[0.021825760289900187]</t>
         </is>
       </c>
       <c r="F87" t="b">
@@ -3152,7 +3152,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>[0.10682922789785951]</t>
+          <t>[0.09864197744635671]</t>
         </is>
       </c>
       <c r="F88" t="b">
@@ -3168,7 +3168,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>[1]</t>
+          <t>[13]</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3183,7 +3183,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>[0.02049497832073982]</t>
+          <t>[0.02129701153948667]</t>
         </is>
       </c>
       <c r="F89" t="b">
@@ -3214,7 +3214,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>[0.04771776805245892]</t>
+          <t>[0.04600140856667701]</t>
         </is>
       </c>
       <c r="F90" t="b">
@@ -3245,7 +3245,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>[0.17924428790117666]</t>
+          <t>[0.16849656838348867]</t>
         </is>
       </c>
       <c r="F91" t="b">
@@ -3261,7 +3261,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3276,7 +3276,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>[0.013058254822632153]</t>
+          <t>[0.011323338188345317]</t>
         </is>
       </c>
       <c r="F92" t="b">
@@ -3307,7 +3307,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>[0.020328983685991273]</t>
+          <t>[0.018802045231517676]</t>
         </is>
       </c>
       <c r="F93" t="b">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>[0.057600277945634534]</t>
+          <t>[0.05466651223522335]</t>
         </is>
       </c>
       <c r="F94" t="b">
@@ -3354,7 +3354,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[7]</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3369,7 +3369,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>[0.032756840998634705]</t>
+          <t>[0.031845023844991896]</t>
         </is>
       </c>
       <c r="F95" t="b">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>[0.04977162021888769]</t>
+          <t>[0.05198533918502164]</t>
         </is>
       </c>
       <c r="F96" t="b">
@@ -3431,7 +3431,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>[0.12703820898379764]</t>
+          <t>[0.1778951004284803]</t>
         </is>
       </c>
       <c r="F97" t="b">
@@ -3447,7 +3447,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3462,7 +3462,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>[0.019578534781652546]</t>
+          <t>[0.017638119909590785]</t>
         </is>
       </c>
       <c r="F98" t="b">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>[0.020121858965089934]</t>
+          <t>[0.02049733697958011]</t>
         </is>
       </c>
       <c r="F99" t="b">
@@ -3524,7 +3524,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>[0.02664051142220302]</t>
+          <t>[0.022976748227021143]</t>
         </is>
       </c>
       <c r="F100" t="b">
@@ -3555,7 +3555,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>[0.2022133893523552]</t>
+          <t>[0.1679835725973545]</t>
         </is>
       </c>
       <c r="F101" t="b">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>[0.1449261581977192]</t>
+          <t>[0.14731334615631708]</t>
         </is>
       </c>
       <c r="F102" t="b">
@@ -3617,7 +3617,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>[0.012632167904844522]</t>
+          <t>[0.013679479562859287]</t>
         </is>
       </c>
       <c r="F103" t="b">
@@ -3648,7 +3648,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>[0.06120174274600509]</t>
+          <t>[0.0701709149255768]</t>
         </is>
       </c>
       <c r="F104" t="b">
@@ -3679,7 +3679,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>[0.049149041739874375]</t>
+          <t>[0.054690816067750544]</t>
         </is>
       </c>
       <c r="F105" t="b">
@@ -3710,7 +3710,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>[0.07382034621909508]</t>
+          <t>[0.08263766949414293]</t>
         </is>
       </c>
       <c r="F106" t="b">
@@ -3741,7 +3741,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>[0.02256390152403482]</t>
+          <t>[0.02014786534439492]</t>
         </is>
       </c>
       <c r="F107" t="b">
@@ -3772,7 +3772,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>[0.07889421035699383]</t>
+          <t>[0.08149224467038735]</t>
         </is>
       </c>
       <c r="F108" t="b">
@@ -3803,7 +3803,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>[0.08045432621881597]</t>
+          <t>[0.0912149768994564]</t>
         </is>
       </c>
       <c r="F109" t="b">
@@ -3834,7 +3834,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>[0.06345525115430277]</t>
+          <t>[0.07204662485197337]</t>
         </is>
       </c>
       <c r="F110" t="b">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>[0.041636581156533306]</t>
+          <t>[0.05683714699367397]</t>
         </is>
       </c>
       <c r="F111" t="b">
@@ -3896,7 +3896,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>[0.04539734320613641]</t>
+          <t>[0.05499771678086548]</t>
         </is>
       </c>
       <c r="F112" t="b">
@@ -3912,7 +3912,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[14]</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3927,7 +3927,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>[0.01857391820223695]</t>
+          <t>[0.01950586998049851]</t>
         </is>
       </c>
       <c r="F113" t="b">
@@ -3958,7 +3958,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>[0.07536883401494748]</t>
+          <t>[0.10205348351845793]</t>
         </is>
       </c>
       <c r="F114" t="b">
@@ -3989,7 +3989,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>[0.09481178964176411]</t>
+          <t>[0.13272651151150994]</t>
         </is>
       </c>
       <c r="F115" t="b">
@@ -4020,7 +4020,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>[0.131532449668759]</t>
+          <t>[0.1914941921380233]</t>
         </is>
       </c>
       <c r="F116" t="b">
@@ -4051,7 +4051,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>[0.05865300264564184]</t>
+          <t>[0.07614146198737799]</t>
         </is>
       </c>
       <c r="F117" t="b">
@@ -4082,7 +4082,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>[0.030001286130499245]</t>
+          <t>[0.03620704464483753]</t>
         </is>
       </c>
       <c r="F118" t="b">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>[0.07643821043479525]</t>
+          <t>[0.10224662584911806]</t>
         </is>
       </c>
       <c r="F119" t="b">
@@ -4144,7 +4144,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>[0.0653506055462148]</t>
+          <t>[0.07416477606674783]</t>
         </is>
       </c>
       <c r="F120" t="b">
@@ -4175,7 +4175,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>[0.015992715104115107]</t>
+          <t>[0.01705592513300936]</t>
         </is>
       </c>
       <c r="F121" t="b">
@@ -4206,7 +4206,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>[0.014021641876944518]</t>
+          <t>[0.015068961546304684]</t>
         </is>
       </c>
       <c r="F122" t="b">
@@ -4237,7 +4237,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>[0.028854421246542597]</t>
+          <t>[0.026201749756025152]</t>
         </is>
       </c>
       <c r="F123" t="b">
@@ -4268,7 +4268,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>[0.036354133806639925]</t>
+          <t>[0.031319007868463825]</t>
         </is>
       </c>
       <c r="F124" t="b">
@@ -4284,7 +4284,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[14]</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -4299,7 +4299,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>[0.015649541037758716]</t>
+          <t>[0.013805884991616122]</t>
         </is>
       </c>
       <c r="F125" t="b">
@@ -4315,7 +4315,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4330,14 +4330,14 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>[0.018156917063604578]</t>
+          <t>[0.018462242637977265]</t>
         </is>
       </c>
       <c r="F126" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G126" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127">
@@ -4361,7 +4361,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>[0.028071992191322653]</t>
+          <t>[0.029418846192570496]</t>
         </is>
       </c>
       <c r="F127" t="b">
@@ -4392,7 +4392,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>[0.05749150639930431]</t>
+          <t>[0.05904190506083551]</t>
         </is>
       </c>
       <c r="F128" t="b">
@@ -4423,7 +4423,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>[0.011657684249587385]</t>
+          <t>[0.011509996216495556]</t>
         </is>
       </c>
       <c r="F129" t="b">
@@ -4454,7 +4454,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>[0.06423754425415147]</t>
+          <t>[0.06357570449739082]</t>
         </is>
       </c>
       <c r="F130" t="b">
@@ -4485,7 +4485,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>[0.06289698459515057]</t>
+          <t>[0.058142459744791805]</t>
         </is>
       </c>
       <c r="F131" t="b">
@@ -4516,7 +4516,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>[0.057017728488025284]</t>
+          <t>[0.056422057759577794]</t>
         </is>
       </c>
       <c r="F132" t="b">
@@ -4547,7 +4547,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>[0.02174384900380812]</t>
+          <t>[0.018997390163875215]</t>
         </is>
       </c>
       <c r="F133" t="b">
@@ -4578,7 +4578,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>[0.028089680262750445]</t>
+          <t>[0.029186057207649614]</t>
         </is>
       </c>
       <c r="F134" t="b">
@@ -4609,7 +4609,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>[0.03313497853709257]</t>
+          <t>[0.03388656621707643]</t>
         </is>
       </c>
       <c r="F135" t="b">
@@ -4640,7 +4640,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>[0.026064753892843733, 0.017535356193679293]</t>
+          <t>[0.02529416260467885, 0.013798905863067697]</t>
         </is>
       </c>
       <c r="F136" t="b">
@@ -4671,7 +4671,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>[0.06206031465962414]</t>
+          <t>[0.06052226969484571]</t>
         </is>
       </c>
       <c r="F137" t="b">
@@ -4702,7 +4702,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>[0.0917851212145329]</t>
+          <t>[0.08254326675001954]</t>
         </is>
       </c>
       <c r="F138" t="b">
@@ -4718,7 +4718,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>[4]</t>
+          <t>[10]</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>[0.03354863470039172]</t>
+          <t>[0.03205765645658193]</t>
         </is>
       </c>
       <c r="F139" t="b">
@@ -4764,7 +4764,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>[0.106540266005709]</t>
+          <t>[0.10880704079452413]</t>
         </is>
       </c>
       <c r="F140" t="b">
@@ -4795,7 +4795,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>[0.010814255331965755]</t>
+          <t>[0.013141757997656999]</t>
         </is>
       </c>
       <c r="F141" t="b">
@@ -4826,7 +4826,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>[0.03744093202661936]</t>
+          <t>[0.034730275159793066]</t>
         </is>
       </c>
       <c r="F142" t="b">
@@ -4842,7 +4842,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -4857,7 +4857,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>[0.02888252594248058]</t>
+          <t>[0.031716229770863344]</t>
         </is>
       </c>
       <c r="F143" t="b">
@@ -4888,7 +4888,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>[0.06374580323427602]</t>
+          <t>[0.05561882393586665]</t>
         </is>
       </c>
       <c r="F144" t="b">
@@ -4919,7 +4919,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>[0.043373369830675676, 0.037242225753304825]</t>
+          <t>[0.04446478199191568, 0.031383593745730055]</t>
         </is>
       </c>
       <c r="F145" t="b">
@@ -4950,7 +4950,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>[0.06942606639637662]</t>
+          <t>[0.05819618583905322]</t>
         </is>
       </c>
       <c r="F146" t="b">
@@ -4981,7 +4981,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>[0.0614683034796615]</t>
+          <t>[0.05419491557774743]</t>
         </is>
       </c>
       <c r="F147" t="b">
@@ -4997,7 +4997,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>[13, 9]</t>
+          <t>[13, 7]</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -5012,14 +5012,14 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>[0.06702657838650405, 0.028132012536679296]</t>
+          <t>[0.06825083243765007, 0.023953432310763044]</t>
         </is>
       </c>
       <c r="F148" t="b">
         <v>0</v>
       </c>
       <c r="G148" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -5043,7 +5043,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>[0.019477331121901385]</t>
+          <t>[0.01905486946496597]</t>
         </is>
       </c>
       <c r="F149" t="b">
@@ -5074,7 +5074,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>[0.04491139691255396]</t>
+          <t>[0.04655570727227314]</t>
         </is>
       </c>
       <c r="F150" t="b">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>[0.022727591032002205]</t>
+          <t>[0.021542299832822326]</t>
         </is>
       </c>
       <c r="F151" t="b">
@@ -5136,7 +5136,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>[0.18847518821355433]</t>
+          <t>[0.17724929404718937]</t>
         </is>
       </c>
       <c r="F152" t="b">
@@ -5167,7 +5167,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>[0.03165782933832325]</t>
+          <t>[0.026636040033248]</t>
         </is>
       </c>
       <c r="F153" t="b">
@@ -5198,7 +5198,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>[0.04545572418058592]</t>
+          <t>[0.060804062840203225]</t>
         </is>
       </c>
       <c r="F154" t="b">
@@ -5229,7 +5229,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>[0.0276689107109876]</t>
+          <t>[0.028956999900583088]</t>
         </is>
       </c>
       <c r="F155" t="b">
@@ -5260,7 +5260,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>[0.027881015029606736]</t>
+          <t>[0.02903778650408317]</t>
         </is>
       </c>
       <c r="F156" t="b">
@@ -5276,29 +5276,29 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
+          <t>[15]</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>protected area effective tool reducing biodiversity loss current legislation distinguishes type marine protected area allowing different level resource extraction theory spatial conservation planning focused identifying notake reserve current approach zoning multiple type protected area result suboptimal plan term protecting biodiversity minimizing negative socioeconomic impact overcame limitation application multizone planning tool marxan zone design network type protected area context california marine life protection act produced zoning configuration entail mean value loss fishery compromising conservation goal spatial numerical optimization tool allows multiple zone outperforms tool identify zone marine reserve way overall impact fishing industry reduced second equitable impact different fishing sector achieved finally examined tradeoff representing biodiversity feature impacting fishery approach applicable marine terrestrial conservation planning delivers ecosystembased management outcome balance conservation industry objective</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
           <t>[14]</t>
         </is>
       </c>
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>protected area effective tool reducing biodiversity loss current legislation distinguishes type marine protected area allowing different level resource extraction theory spatial conservation planning focused identifying notake reserve current approach zoning multiple type protected area result suboptimal plan term protecting biodiversity minimizing negative socioeconomic impact overcame limitation application multizone planning tool marxan zone design network type protected area context california marine life protection act produced zoning configuration entail mean value loss fishery compromising conservation goal spatial numerical optimization tool allows multiple zone outperforms tool identify zone marine reserve way overall impact fishing industry reduced second equitable impact different fishing sector achieved finally examined tradeoff representing biodiversity feature impacting fishery approach applicable marine terrestrial conservation planning delivers ecosystembased management outcome balance conservation industry objective</t>
-        </is>
-      </c>
-      <c r="D157" t="inlineStr">
-        <is>
-          <t>[14]</t>
-        </is>
-      </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>[0.09604065767381369]</t>
+          <t>[0.1349617170817047]</t>
         </is>
       </c>
       <c r="F157" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G157" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158">
@@ -5322,7 +5322,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>[0.0407107363888122]</t>
+          <t>[0.046648500199581104]</t>
         </is>
       </c>
       <c r="F158" t="b">
@@ -5353,7 +5353,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>[0.04617649895773118]</t>
+          <t>[0.05342525266545209]</t>
         </is>
       </c>
       <c r="F159" t="b">
@@ -5384,7 +5384,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>[0.03796788836639916]</t>
+          <t>[0.04476771339314058]</t>
         </is>
       </c>
       <c r="F160" t="b">
@@ -5415,7 +5415,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>[0.09876391070825966]</t>
+          <t>[0.12344694315036071]</t>
         </is>
       </c>
       <c r="F161" t="b">
@@ -5446,7 +5446,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>[0.029764974494070468]</t>
+          <t>[0.03453510542315903]</t>
         </is>
       </c>
       <c r="F162" t="b">
@@ -5477,7 +5477,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>[0.052578151668986016]</t>
+          <t>[0.052820172924846746]</t>
         </is>
       </c>
       <c r="F163" t="b">
@@ -5508,7 +5508,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>[0.05955765983101318]</t>
+          <t>[0.05854474161963208]</t>
         </is>
       </c>
       <c r="F164" t="b">
@@ -5539,7 +5539,7 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>[0.017557784136226346]</t>
+          <t>[0.013361515549092408]</t>
         </is>
       </c>
       <c r="F165" t="b">
@@ -5570,7 +5570,7 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>[0.029792032294228447]</t>
+          <t>[0.03048782449091932]</t>
         </is>
       </c>
       <c r="F166" t="b">

</xml_diff>